<commit_message>
Implemented some unit tests
</commit_message>
<xml_diff>
--- a/doc/database.xlsx
+++ b/doc/database.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\heins\GitHub\Build\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="48" windowWidth="17124" windowHeight="7968" activeTab="1"/>
+    <workbookView xWindow="2340" yWindow="45" windowWidth="17130" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -23,12 +28,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fields!$A$4:$I$76</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="179">
   <si>
     <t>Stored data</t>
   </si>
@@ -516,9 +521,6 @@
     <t>p1, p2, date, file, NT range, 5=5=4=2, NAT/PREC/OTHER</t>
   </si>
   <si>
-    <t>p1, p2, date, file, lead, UDCA, …</t>
-  </si>
-  <si>
     <t>files</t>
   </si>
   <si>
@@ -535,6 +537,39 @@
   </si>
   <si>
     <t xml:space="preserve">    but +26-52 on errors, 10 on tableau</t>
+  </si>
+  <si>
+    <t>handle2</t>
+  </si>
+  <si>
+    <t>handleBBO</t>
+  </si>
+  <si>
+    <t>handle3</t>
+  </si>
+  <si>
+    <t>displayName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>addition</t>
+  </si>
+  <si>
+    <t>countryCode</t>
+  </si>
+  <si>
+    <t>Need a way to do approximate matching.</t>
+  </si>
+  <si>
+    <t>Would like to be able to merge two players.</t>
+  </si>
+  <si>
+    <t>p1, p2, date, file, lead '(NT and suit), UDCA, …</t>
   </si>
 </sst>
 </file>
@@ -645,14 +680,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -690,9 +728,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -727,7 +765,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -762,7 +800,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -942,22 +980,22 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" style="4" customWidth="1"/>
-    <col min="5" max="6" width="5.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="4" customWidth="1"/>
+    <col min="5" max="6" width="5.375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.875" style="4" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="26.5546875" customWidth="1"/>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -968,7 +1006,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -977,7 +1015,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1006,7 +1044,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1033,7 +1071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1060,7 +1098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1090,7 +1128,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1118,7 +1156,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1146,7 +1184,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
@@ -1174,7 +1212,7 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1204,7 +1242,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1234,7 +1272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>1</v>
       </c>
@@ -1262,7 +1300,7 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>1</v>
       </c>
@@ -1292,7 +1330,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1322,7 +1360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1350,7 +1388,7 @@
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1380,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1407,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1435,7 +1473,7 @@
       </c>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1460,7 +1498,7 @@
       </c>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1485,7 +1523,7 @@
       </c>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1510,7 +1548,7 @@
       </c>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1538,7 +1576,7 @@
       </c>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>27</v>
       </c>
@@ -1565,7 +1603,7 @@
       </c>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1593,7 +1631,7 @@
       </c>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1618,7 +1656,7 @@
       </c>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1643,7 +1681,7 @@
       </c>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1668,7 +1706,7 @@
       </c>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -1696,7 +1734,7 @@
       </c>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>59</v>
       </c>
@@ -1724,7 +1762,7 @@
       </c>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -1753,7 +1791,7 @@
       </c>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -1782,7 +1820,7 @@
       </c>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -1810,7 +1848,7 @@
       </c>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -1840,7 +1878,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -1870,7 +1908,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>72</v>
       </c>
@@ -1896,7 +1934,7 @@
       <c r="H36" s="7"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>72</v>
       </c>
@@ -1923,7 +1961,7 @@
       </c>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1948,7 +1986,7 @@
       </c>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -1976,7 +2014,7 @@
       </c>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>72</v>
       </c>
@@ -2003,7 +2041,7 @@
       </c>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>72</v>
       </c>
@@ -2030,7 +2068,7 @@
       </c>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -2055,7 +2093,7 @@
       </c>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -2080,7 +2118,7 @@
       </c>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2105,7 +2143,7 @@
       </c>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>72</v>
       </c>
@@ -2130,7 +2168,7 @@
       <c r="H45" s="7"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -2152,7 +2190,7 @@
       </c>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -2180,7 +2218,7 @@
       </c>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -2205,7 +2243,7 @@
       </c>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -2230,7 +2268,7 @@
       </c>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -2255,7 +2293,7 @@
       </c>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -2283,7 +2321,7 @@
       </c>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -2308,7 +2346,7 @@
       </c>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>103</v>
       </c>
@@ -2320,7 +2358,7 @@
       </c>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -2349,7 +2387,7 @@
       </c>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -2378,7 +2416,7 @@
       </c>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>103</v>
       </c>
@@ -2399,7 +2437,7 @@
       </c>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -2427,7 +2465,7 @@
       </c>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -2455,7 +2493,7 @@
       </c>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>112</v>
       </c>
@@ -2480,7 +2518,7 @@
       </c>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -2505,7 +2543,7 @@
       </c>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>112</v>
       </c>
@@ -2530,7 +2568,7 @@
       </c>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>117</v>
       </c>
@@ -2558,7 +2596,7 @@
       </c>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>120</v>
       </c>
@@ -2584,7 +2622,7 @@
       </c>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -2609,7 +2647,7 @@
       </c>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>123</v>
       </c>
@@ -2631,7 +2669,7 @@
       </c>
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>123</v>
       </c>
@@ -2657,7 +2695,7 @@
       </c>
       <c r="I66" s="6"/>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>125</v>
       </c>
@@ -2679,7 +2717,7 @@
       </c>
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>125</v>
       </c>
@@ -2705,7 +2743,7 @@
       </c>
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>125</v>
       </c>
@@ -2730,7 +2768,7 @@
       </c>
       <c r="I69" s="6"/>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>125</v>
       </c>
@@ -2755,7 +2793,7 @@
       </c>
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>125</v>
       </c>
@@ -2780,7 +2818,7 @@
       </c>
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>126</v>
       </c>
@@ -2802,7 +2840,7 @@
       </c>
       <c r="I72" s="6"/>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>126</v>
       </c>
@@ -2827,7 +2865,7 @@
       </c>
       <c r="I73" s="6"/>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>126</v>
       </c>
@@ -2852,7 +2890,7 @@
       </c>
       <c r="I74" s="6"/>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>126</v>
       </c>
@@ -2877,7 +2915,7 @@
       </c>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>109</v>
       </c>
@@ -2923,11 +2961,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2944,11 +2982,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2967,11 +3005,11 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2987,22 +3025,22 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.75" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.75" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -3019,7 +3057,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -3039,10 +3077,10 @@
         <v>194.549560546875</v>
       </c>
       <c r="F5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -3062,10 +3100,10 @@
         <v>15.735626220703125</v>
       </c>
       <c r="F6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -3085,7 +3123,7 @@
         <v>62.75177001953125</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -3105,7 +3143,7 @@
         <v>3.4332275390625</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -3125,7 +3163,7 @@
         <v>45.7763671875</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -3145,7 +3183,7 @@
         <v>6.103515625</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>142</v>
       </c>
@@ -3156,42 +3194,42 @@
         <v>328.35006713867187</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>159</v>
       </c>
@@ -3199,12 +3237,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>160</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3217,15 +3255,72 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3242,9 +3337,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>152</v>
       </c>
@@ -3263,9 +3358,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>153</v>
       </c>
@@ -3284,9 +3379,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>154</v>
       </c>
@@ -3305,9 +3400,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>155</v>
       </c>
@@ -3326,9 +3421,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>156</v>
       </c>
@@ -3349,11 +3444,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>